<commit_message>
Update catalog with correct parcel link
</commit_message>
<xml_diff>
--- a/references/Zoning_Parser_Invalids.xlsx
+++ b/references/Zoning_Parser_Invalids.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="not_parsed" sheetId="1" r:id="rId1"/>
     <sheet name="invalid_zone" sheetId="2" r:id="rId2"/>
     <sheet name="invalid_height" sheetId="3" r:id="rId3"/>
     <sheet name="invalid_overlay" sheetId="4" r:id="rId4"/>
+    <sheet name="examples" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">examples!$A$1:$C$45</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="265">
   <si>
     <t>ZONE_CMPLT</t>
   </si>
@@ -904,19 +908,27 @@
   <si>
     <t>GW</t>
   </si>
+  <si>
+    <t>ZONE_CMPLT (not parsed)</t>
+  </si>
+  <si>
+    <t>INVALID_ZONE</t>
+  </si>
+  <si>
+    <t>INVALID_STRINGS</t>
+  </si>
+  <si>
+    <t>INVALID_HEIGHT</t>
+  </si>
+  <si>
+    <t>INVALID_OVERLAY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,7 +945,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -958,8 +970,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -967,14 +997,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -999,6 +1044,53 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1282,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1551,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>7</v>
       </c>
@@ -1469,7 +1561,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>79</v>
       </c>
@@ -1762,17 +1854,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>24</v>
       </c>
@@ -1787,7 +1879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>27</v>
       </c>
@@ -1817,7 +1909,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>31</v>
       </c>
@@ -1837,7 +1929,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>32</v>
       </c>
@@ -1907,7 +1999,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1916,7 +2008,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2161,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2077,7 +2170,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="A13" activeCellId="1" sqref="A4:A6 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,6 +2315,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2229,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,6 +2682,307 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="21"/>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="23"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="23"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="23"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B21" s="23"/>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="23"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="23"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="23"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="23"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="23"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="23"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="23"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="23"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="23"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="23"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" s="23"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="23"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="23"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="23"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="23"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B41" s="23"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>